<commit_message>
Mise à jour site panneaux rocko
</commit_message>
<xml_diff>
--- a/prix/prix.xlsx
+++ b/prix/prix.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Nouveau dossier\prix\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\rocko\prix\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{63097933-5688-4D5E-89EE-07C063DA5938}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A2BB0B94-7D46-445D-A6D1-E15BB67D0416}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{6E95DC93-531D-460D-9A06-44397A8920D7}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="33">
   <si>
     <t>path</t>
   </si>
@@ -114,6 +114,27 @@
   </si>
   <si>
     <t>ROCKO 1230X2800 GREIGE BABYLON 130</t>
+  </si>
+  <si>
+    <t>galerie/K190.jpg</t>
+  </si>
+  <si>
+    <t>galerie/K365.jpg</t>
+  </si>
+  <si>
+    <t>galerie/K551.jpg</t>
+  </si>
+  <si>
+    <t>galerie/R109.jpg</t>
+  </si>
+  <si>
+    <t>galerie/R120.jpg</t>
+  </si>
+  <si>
+    <t>galerie/R160.jpg</t>
+  </si>
+  <si>
+    <t>galerie/R162B.jpg</t>
   </si>
 </sst>
 </file>
@@ -616,7 +637,7 @@
   <dimension ref="A1:G448"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScale="98" zoomScaleNormal="98" workbookViewId="0">
-      <selection activeCell="B17" sqref="B17"/>
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -669,7 +690,9 @@
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A3" s="12"/>
+      <c r="A3" s="12" t="s">
+        <v>32</v>
+      </c>
       <c r="B3" s="27" t="s">
         <v>9</v>
       </c>
@@ -685,7 +708,9 @@
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A4" s="12"/>
+      <c r="A4" s="12" t="s">
+        <v>26</v>
+      </c>
       <c r="B4" s="27" t="s">
         <v>11</v>
       </c>
@@ -701,7 +726,9 @@
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A5" s="12"/>
+      <c r="A5" s="12" t="s">
+        <v>30</v>
+      </c>
       <c r="B5" s="27" t="s">
         <v>13</v>
       </c>
@@ -717,7 +744,9 @@
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A6" s="12"/>
+      <c r="A6" s="12" t="s">
+        <v>28</v>
+      </c>
       <c r="B6" s="27" t="s">
         <v>15</v>
       </c>
@@ -733,7 +762,9 @@
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A7" s="12"/>
+      <c r="A7" s="12" t="s">
+        <v>31</v>
+      </c>
       <c r="B7" s="27" t="s">
         <v>17</v>
       </c>
@@ -765,7 +796,9 @@
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A9" s="12"/>
+      <c r="A9" s="12" t="s">
+        <v>27</v>
+      </c>
       <c r="B9" s="27" t="s">
         <v>21</v>
       </c>
@@ -781,7 +814,9 @@
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A10" s="12"/>
+      <c r="A10" s="12" t="s">
+        <v>29</v>
+      </c>
       <c r="B10" s="27" t="s">
         <v>23</v>
       </c>

</xml_diff>